<commit_message>
snohomish scraper coordinator done
</commit_message>
<xml_diff>
--- a/server/Auction_Notes_2022.xlsx
+++ b/server/Auction_Notes_2022.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcouch/Documents/CODE/react_testing/tax_auction/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E2FBA2-7C06-4D48-9621-7527FB1AD6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A50CE19-DAC2-CB4C-B209-DF355FD49D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="AuctionNotes" sheetId="1" r:id="rId1"/>
-    <sheet name="Snohomish" sheetId="2" r:id="rId2"/>
+    <sheet name="ParcelList" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="89">
   <si>
     <t>COUNTY</t>
   </si>
@@ -57,23 +57,260 @@
     <t>Snohomish</t>
   </si>
   <si>
-    <t>sample url</t>
-  </si>
-  <si>
-    <t>fake url</t>
-  </si>
-  <si>
     <t>https://www.bid4assets.com</t>
   </si>
   <si>
+    <t>https://snohomishcountywa.gov/220/Tax-Foreclosures</t>
+  </si>
+  <si>
+    <t>AUCTION_SITE_FLAG</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>PARCEL_DATA_BASE_URL</t>
+  </si>
+  <si>
+    <t>https://www.snoco.org/proptax/search.aspx?parcel_number=</t>
+  </si>
+  <si>
+    <t>PARCEL_VIEWER_URL</t>
+  </si>
+  <si>
+    <t>https://scopi.snoco.org/Html5Viewer/Index.html?configBase=https://scopi.snoco.org/Geocortex/Essentials/REST/sites/SCOPI/viewers/SCOPI/virtualdirectory/Resources/Config/Default</t>
+  </si>
+  <si>
+    <t>https://www.snohomishcountywa.gov/3399/Requests-For-Foreclosure-Information</t>
+  </si>
+  <si>
+    <t>12/6/2022</t>
+  </si>
+  <si>
+    <t>PARCEL_NUM</t>
+  </si>
+  <si>
+    <t>00373301100301</t>
+  </si>
+  <si>
+    <t>00373301100305</t>
+  </si>
+  <si>
+    <t>00377801300100</t>
+  </si>
+  <si>
+    <t>00377801400100</t>
+  </si>
+  <si>
+    <t>00397700001001</t>
+  </si>
+  <si>
+    <t>00403800006701</t>
+  </si>
+  <si>
+    <t>00422800000300</t>
+  </si>
+  <si>
+    <t>00422800000400</t>
+  </si>
+  <si>
+    <t>00422800000500</t>
+  </si>
+  <si>
+    <t>00452500000100</t>
+  </si>
+  <si>
+    <t>00460100003900</t>
+  </si>
+  <si>
+    <t>00486300000801</t>
+  </si>
+  <si>
+    <t>00486300000806</t>
+  </si>
+  <si>
+    <t>00489200001600</t>
+  </si>
+  <si>
+    <t>00489200001700</t>
+  </si>
+  <si>
+    <t>00493900006304</t>
+  </si>
+  <si>
+    <t>00543600001900</t>
+  </si>
+  <si>
+    <t>00544700100100</t>
+  </si>
+  <si>
+    <t>00556800101802</t>
+  </si>
+  <si>
+    <t>00557100406000</t>
+  </si>
+  <si>
+    <t>00557100406100</t>
+  </si>
+  <si>
+    <t>00557500003202</t>
+  </si>
+  <si>
+    <t>00602900002000</t>
+  </si>
+  <si>
+    <t>00608200700100</t>
+  </si>
+  <si>
+    <t>00611100007300</t>
+  </si>
+  <si>
+    <t>00622400000600</t>
+  </si>
+  <si>
+    <t>00645300000200</t>
+  </si>
+  <si>
+    <t>00647500006300</t>
+  </si>
+  <si>
+    <t>00667400003200</t>
+  </si>
+  <si>
+    <t>00818700010300</t>
+  </si>
+  <si>
+    <t>00857312810200</t>
+  </si>
+  <si>
+    <t>00861100001100</t>
+  </si>
+  <si>
+    <t>01013600001000</t>
+  </si>
+  <si>
+    <t>01026900200800</t>
+  </si>
+  <si>
+    <t>01017100000200</t>
+  </si>
+  <si>
+    <t>01051600510100</t>
+  </si>
+  <si>
+    <t>01065600000200</t>
+  </si>
+  <si>
+    <t>01070900031000</t>
+  </si>
+  <si>
+    <t>27041900108900</t>
+  </si>
+  <si>
+    <t>27043300302900</t>
+  </si>
+  <si>
+    <t>27052600401200</t>
+  </si>
+  <si>
+    <t>27090800201200</t>
+  </si>
+  <si>
+    <t>28050100404700</t>
+  </si>
+  <si>
+    <t>28061400400300</t>
+  </si>
+  <si>
+    <t>28061800100100</t>
+  </si>
+  <si>
+    <t>28062200402000</t>
+  </si>
+  <si>
+    <t>28083300304600</t>
+  </si>
+  <si>
+    <t>30060600201400</t>
+  </si>
+  <si>
+    <t>30062000402000</t>
+  </si>
+  <si>
+    <t>30080700100800</t>
+  </si>
+  <si>
+    <t>30080700102600</t>
+  </si>
+  <si>
+    <t>31042100303900</t>
+  </si>
+  <si>
+    <t>31050900200300</t>
+  </si>
+  <si>
+    <t>31052500103500</t>
+  </si>
+  <si>
+    <t>31060700400500</t>
+  </si>
+  <si>
+    <t>31061800202400</t>
+  </si>
+  <si>
+    <t>31063200101500</t>
+  </si>
+  <si>
+    <t>32031200400500</t>
+  </si>
+  <si>
+    <t>32042600301800</t>
+  </si>
+  <si>
+    <t>32043500200900</t>
+  </si>
+  <si>
+    <t>32052800100100</t>
+  </si>
+  <si>
+    <t>32052800100101</t>
+  </si>
+  <si>
+    <t>32052800101300</t>
+  </si>
+  <si>
+    <t>32063200101700</t>
+  </si>
+  <si>
+    <t>32090500402100</t>
+  </si>
+  <si>
+    <t>32092300103000</t>
+  </si>
+  <si>
+    <t>32092400201300</t>
+  </si>
+  <si>
+    <t>DATE_UPDATED</t>
+  </si>
+  <si>
+    <t>11/3/2022</t>
+  </si>
+  <si>
     <t>King</t>
+  </si>
+  <si>
+    <t>9/12/22</t>
+  </si>
+  <si>
+    <t>sample</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +322,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,8 +356,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,25 +673,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8B109A-2724-4740-B131-3DE7DE546852}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -458,47 +704,74 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>44877</v>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44816</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{54597207-3B0D-6949-8151-5927A023F3BD}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{7EDFF233-C192-6E47-8667-1C7A690C3979}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{A74CA47F-5F8E-444A-81BD-A214D2C9EC49}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{3456EF92-C537-B04F-B24A-4963B3B8DF33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -506,66 +779,772 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45ED94-1D31-3149-A41C-8E0A68424B78}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
King County scraped basic, land, and tax
</commit_message>
<xml_diff>
--- a/server/Auction_Notes_2022.xlsx
+++ b/server/Auction_Notes_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcouch/Documents/CODE/react_testing/tax_auction/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A50CE19-DAC2-CB4C-B209-DF355FD49D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2DF8D3-A8C1-4A4E-A8FC-7BFFCC26946D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="AuctionNotes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="298">
   <si>
     <t>COUNTY</t>
   </si>
@@ -300,17 +300,644 @@
     <t>King</t>
   </si>
   <si>
-    <t>9/12/22</t>
-  </si>
-  <si>
-    <t>sample</t>
+    <t>https://kingcounty.gov/depts/finance-business-operations/treasury/foreclosure.aspx</t>
+  </si>
+  <si>
+    <t>12/26/2022</t>
+  </si>
+  <si>
+    <t>1021069089</t>
+  </si>
+  <si>
+    <t>1024069112</t>
+  </si>
+  <si>
+    <t>1157200100</t>
+  </si>
+  <si>
+    <t>1218000075</t>
+  </si>
+  <si>
+    <t>1223049030</t>
+  </si>
+  <si>
+    <t>1252200170</t>
+  </si>
+  <si>
+    <t>1311600090</t>
+  </si>
+  <si>
+    <t>1312200160</t>
+  </si>
+  <si>
+    <t>1322059140</t>
+  </si>
+  <si>
+    <t>1364300565</t>
+  </si>
+  <si>
+    <t>1370802919</t>
+  </si>
+  <si>
+    <t>1423049037</t>
+  </si>
+  <si>
+    <t>1447200120</t>
+  </si>
+  <si>
+    <t>1550000410</t>
+  </si>
+  <si>
+    <t>1622049170</t>
+  </si>
+  <si>
+    <t>1623049169</t>
+  </si>
+  <si>
+    <t>1623049345</t>
+  </si>
+  <si>
+    <t>1701000300</t>
+  </si>
+  <si>
+    <t>1704900520</t>
+  </si>
+  <si>
+    <t>1724500040</t>
+  </si>
+  <si>
+    <t>1742900010</t>
+  </si>
+  <si>
+    <t>1773100490</t>
+  </si>
+  <si>
+    <t>1789400670</t>
+  </si>
+  <si>
+    <t>1817800010</t>
+  </si>
+  <si>
+    <t>1822119015</t>
+  </si>
+  <si>
+    <t>1823059262</t>
+  </si>
+  <si>
+    <t>1830700120</t>
+  </si>
+  <si>
+    <t>1841400120</t>
+  </si>
+  <si>
+    <t>1920079032</t>
+  </si>
+  <si>
+    <t>1939130350</t>
+  </si>
+  <si>
+    <t>2022059259</t>
+  </si>
+  <si>
+    <t>2114300050</t>
+  </si>
+  <si>
+    <t>2135200180</t>
+  </si>
+  <si>
+    <t>2144800615</t>
+  </si>
+  <si>
+    <t>2144800851</t>
+  </si>
+  <si>
+    <t>2185000495</t>
+  </si>
+  <si>
+    <t>2188203645</t>
+  </si>
+  <si>
+    <t>2221069022</t>
+  </si>
+  <si>
+    <t>2221069059</t>
+  </si>
+  <si>
+    <t>2296500100</t>
+  </si>
+  <si>
+    <t>2361000160</t>
+  </si>
+  <si>
+    <t>2422079028</t>
+  </si>
+  <si>
+    <t>2423029214</t>
+  </si>
+  <si>
+    <t>2425069083</t>
+  </si>
+  <si>
+    <t>2426059036</t>
+  </si>
+  <si>
+    <t>2516000500</t>
+  </si>
+  <si>
+    <t>2523039047</t>
+  </si>
+  <si>
+    <t>2524059275</t>
+  </si>
+  <si>
+    <t>2720069031</t>
+  </si>
+  <si>
+    <t>2770601335</t>
+  </si>
+  <si>
+    <t>2822049102</t>
+  </si>
+  <si>
+    <t>2824069011</t>
+  </si>
+  <si>
+    <t>2824069210</t>
+  </si>
+  <si>
+    <t>2824069397</t>
+  </si>
+  <si>
+    <t>2840200520</t>
+  </si>
+  <si>
+    <t>2840200525</t>
+  </si>
+  <si>
+    <t>2840200530</t>
+  </si>
+  <si>
+    <t>2883201155</t>
+  </si>
+  <si>
+    <t>2924069017</t>
+  </si>
+  <si>
+    <t>2937600770</t>
+  </si>
+  <si>
+    <t>2946001000</t>
+  </si>
+  <si>
+    <t>2976800935</t>
+  </si>
+  <si>
+    <t>3013301450</t>
+  </si>
+  <si>
+    <t>3023000490</t>
+  </si>
+  <si>
+    <t>3083000745</t>
+  </si>
+  <si>
+    <t>3211530750</t>
+  </si>
+  <si>
+    <t>3221049033</t>
+  </si>
+  <si>
+    <t>3223059203</t>
+  </si>
+  <si>
+    <t>3223069032</t>
+  </si>
+  <si>
+    <t>3223069121</t>
+  </si>
+  <si>
+    <t>3226200085</t>
+  </si>
+  <si>
+    <t>3256400070</t>
+  </si>
+  <si>
+    <t>3300701580</t>
+  </si>
+  <si>
+    <t>3300780040</t>
+  </si>
+  <si>
+    <t>3333002170</t>
+  </si>
+  <si>
+    <t>3339400325</t>
+  </si>
+  <si>
+    <t>3343301023</t>
+  </si>
+  <si>
+    <t>3345100371</t>
+  </si>
+  <si>
+    <t>3352401755</t>
+  </si>
+  <si>
+    <t>3361401800</t>
+  </si>
+  <si>
+    <t>3394200590</t>
+  </si>
+  <si>
+    <t>3422059172</t>
+  </si>
+  <si>
+    <t>3451000415</t>
+  </si>
+  <si>
+    <t>3459800240</t>
+  </si>
+  <si>
+    <t>3496500210</t>
+  </si>
+  <si>
+    <t>3523069021</t>
+  </si>
+  <si>
+    <t>3523069148</t>
+  </si>
+  <si>
+    <t>3523069177</t>
+  </si>
+  <si>
+    <t>3575303820</t>
+  </si>
+  <si>
+    <t>3623000170</t>
+  </si>
+  <si>
+    <t>3626039007</t>
+  </si>
+  <si>
+    <t>3750606450</t>
+  </si>
+  <si>
+    <t>3751606207</t>
+  </si>
+  <si>
+    <t>3793600190</t>
+  </si>
+  <si>
+    <t>3793800440</t>
+  </si>
+  <si>
+    <t>3800910150</t>
+  </si>
+  <si>
+    <t>3828000490</t>
+  </si>
+  <si>
+    <t>3828000495</t>
+  </si>
+  <si>
+    <t>3876201500</t>
+  </si>
+  <si>
+    <t>3892300130</t>
+  </si>
+  <si>
+    <t>3992700305</t>
+  </si>
+  <si>
+    <t>4008400015</t>
+  </si>
+  <si>
+    <t>4014400207</t>
+  </si>
+  <si>
+    <t>4014400211</t>
+  </si>
+  <si>
+    <t>4046501030</t>
+  </si>
+  <si>
+    <t>4047900030</t>
+  </si>
+  <si>
+    <t>4051170360</t>
+  </si>
+  <si>
+    <t>4058200390</t>
+  </si>
+  <si>
+    <t>4059400710</t>
+  </si>
+  <si>
+    <t>4060000500</t>
+  </si>
+  <si>
+    <t>4123840720</t>
+  </si>
+  <si>
+    <t>4127000902</t>
+  </si>
+  <si>
+    <t>4202401070</t>
+  </si>
+  <si>
+    <t>4219600230</t>
+  </si>
+  <si>
+    <t>4303200360</t>
+  </si>
+  <si>
+    <t>4458740470</t>
+  </si>
+  <si>
+    <t>5153650040</t>
+  </si>
+  <si>
+    <t>5379800704</t>
+  </si>
+  <si>
+    <t>5379802310</t>
+  </si>
+  <si>
+    <t>5381000395</t>
+  </si>
+  <si>
+    <t>5514600050</t>
+  </si>
+  <si>
+    <t>5554200400</t>
+  </si>
+  <si>
+    <t>5561400420</t>
+  </si>
+  <si>
+    <t>5680001115</t>
+  </si>
+  <si>
+    <t>5683500035</t>
+  </si>
+  <si>
+    <t>5702200070</t>
+  </si>
+  <si>
+    <t>6082400182</t>
+  </si>
+  <si>
+    <t>6083000127</t>
+  </si>
+  <si>
+    <t>6150200020</t>
+  </si>
+  <si>
+    <t>6381501605</t>
+  </si>
+  <si>
+    <t>6383500750</t>
+  </si>
+  <si>
+    <t>6395500450</t>
+  </si>
+  <si>
+    <t>6711000190</t>
+  </si>
+  <si>
+    <t>6746702015</t>
+  </si>
+  <si>
+    <t>6788201825</t>
+  </si>
+  <si>
+    <t>6798100595</t>
+  </si>
+  <si>
+    <t>6905200025</t>
+  </si>
+  <si>
+    <t>7129301575</t>
+  </si>
+  <si>
+    <t>7177300685</t>
+  </si>
+  <si>
+    <t>7231600445</t>
+  </si>
+  <si>
+    <t>7231600460</t>
+  </si>
+  <si>
+    <t>7290300370</t>
+  </si>
+  <si>
+    <t>7305300115</t>
+  </si>
+  <si>
+    <t>7334800190</t>
+  </si>
+  <si>
+    <t>7338401370</t>
+  </si>
+  <si>
+    <t>7398901090</t>
+  </si>
+  <si>
+    <t>7436000135</t>
+  </si>
+  <si>
+    <t>7450800050</t>
+  </si>
+  <si>
+    <t>7518500500</t>
+  </si>
+  <si>
+    <t>7518505540</t>
+  </si>
+  <si>
+    <t>7577700201</t>
+  </si>
+  <si>
+    <t>7649900046</t>
+  </si>
+  <si>
+    <t>7681100020</t>
+  </si>
+  <si>
+    <t>7682800247</t>
+  </si>
+  <si>
+    <t>7754100370</t>
+  </si>
+  <si>
+    <t>7787890400</t>
+  </si>
+  <si>
+    <t>7801300160</t>
+  </si>
+  <si>
+    <t>7818900130</t>
+  </si>
+  <si>
+    <t>7861000132</t>
+  </si>
+  <si>
+    <t>7883600961</t>
+  </si>
+  <si>
+    <t>7883606755</t>
+  </si>
+  <si>
+    <t>7950302015</t>
+  </si>
+  <si>
+    <t>8018600411</t>
+  </si>
+  <si>
+    <t>8018600415</t>
+  </si>
+  <si>
+    <t>8018600420</t>
+  </si>
+  <si>
+    <t>8018600422</t>
+  </si>
+  <si>
+    <t>8046000110</t>
+  </si>
+  <si>
+    <t>8121220790</t>
+  </si>
+  <si>
+    <t>8130200750</t>
+  </si>
+  <si>
+    <t>8651510590</t>
+  </si>
+  <si>
+    <t>8656800240</t>
+  </si>
+  <si>
+    <t>8844300100</t>
+  </si>
+  <si>
+    <t>8856002186</t>
+  </si>
+  <si>
+    <t>8856004380</t>
+  </si>
+  <si>
+    <t>8898530450</t>
+  </si>
+  <si>
+    <t>8928100090</t>
+  </si>
+  <si>
+    <t>8944270150</t>
+  </si>
+  <si>
+    <t>9134200070</t>
+  </si>
+  <si>
+    <t>9183702835</t>
+  </si>
+  <si>
+    <t>9188620230</t>
+  </si>
+  <si>
+    <t>9264960070</t>
+  </si>
+  <si>
+    <t>9290850890</t>
+  </si>
+  <si>
+    <t>9320900230</t>
+  </si>
+  <si>
+    <t>9382200095</t>
+  </si>
+  <si>
+    <t>9382200096</t>
+  </si>
+  <si>
+    <t>9428500072</t>
+  </si>
+  <si>
+    <t>9428500073</t>
+  </si>
+  <si>
+    <t>9459200085</t>
+  </si>
+  <si>
+    <t>9828702296</t>
+  </si>
+  <si>
+    <t>9834200775</t>
+  </si>
+  <si>
+    <t>0024500320</t>
+  </si>
+  <si>
+    <t>0100601160</t>
+  </si>
+  <si>
+    <t>0182000349</t>
+  </si>
+  <si>
+    <t>0193800140</t>
+  </si>
+  <si>
+    <t>0303000450</t>
+  </si>
+  <si>
+    <t>0324500780</t>
+  </si>
+  <si>
+    <t>0380000950</t>
+  </si>
+  <si>
+    <t>0643400060</t>
+  </si>
+  <si>
+    <t>0722059047</t>
+  </si>
+  <si>
+    <t>0742000052</t>
+  </si>
+  <si>
+    <t>0758000010</t>
+  </si>
+  <si>
+    <t>0832000140</t>
+  </si>
+  <si>
+    <t>0872000090</t>
+  </si>
+  <si>
+    <t>0923049112</t>
+  </si>
+  <si>
+    <t>0923049436</t>
+  </si>
+  <si>
+    <t>https://kingcounty.gov/depts/finance-business-operations/treasury/foreclosure/current-foreclosure-action/foreclosure-properties.aspx</t>
+  </si>
+  <si>
+    <t>https://blue.kingcounty.com/Assessor/eRealProperty/Dashboard.aspx?ParcelNbr=</t>
+  </si>
+  <si>
+    <t>https://gismaps.kingcounty.gov/parcelviewer2//?pin=</t>
+  </si>
+  <si>
+    <t>9/13/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +955,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF23221F"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -354,10 +994,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8B109A-2724-4740-B131-3DE7DE546852}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,19 +1389,19 @@
         <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>294</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>88</v>
+        <v>295</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -772,6 +1414,7 @@
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{A74CA47F-5F8E-444A-81BD-A214D2C9EC49}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{3456EF92-C537-B04F-B24A-4963B3B8DF33}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{20A4526F-F7E4-874C-B6C1-AD92A24BF129}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -779,9 +1422,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45ED94-1D31-3149-A41C-8E0A68424B78}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:B274"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1543,6 +2188,2272 @@
         <v>85</v>
       </c>
     </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>86</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>86</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>86</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>86</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>86</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>86</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>86</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>86</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>86</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>86</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>86</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>86</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>86</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>86</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>86</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>86</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>86</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>86</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>86</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>86</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>86</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>86</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>86</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>86</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>86</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>86</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>86</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>86</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>86</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>86</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>86</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>86</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>86</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>86</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>86</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>86</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>86</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>86</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>86</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>86</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>86</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>86</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>86</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>86</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>86</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>86</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>86</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>86</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>86</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>86</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>86</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>86</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>86</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>86</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>86</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>86</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>86</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>86</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>86</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>86</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>86</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>86</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>86</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>86</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>86</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>86</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>86</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>86</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>86</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>86</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>86</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>86</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>86</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>86</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>86</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>86</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>86</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>86</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>86</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>86</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>86</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>86</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>86</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>86</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>86</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>86</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>86</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>86</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>86</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>86</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>86</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>86</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>86</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>86</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>86</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>86</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>86</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>86</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>86</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>86</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>86</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>86</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>86</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>86</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>86</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>86</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>86</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>86</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>86</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>86</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>86</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>86</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>86</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>86</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>86</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>86</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>86</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>86</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>86</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>86</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>86</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>86</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>86</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>86</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>86</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>86</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>86</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>86</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>86</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>86</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>86</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>86</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>86</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>86</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>86</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>86</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>86</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>86</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>86</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>86</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>86</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>86</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>86</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>86</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>86</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>86</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>86</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>86</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>86</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>86</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>86</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>86</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>86</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>86</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>86</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>86</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>86</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>86</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>86</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>86</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>86</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>86</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>86</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>86</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>86</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>86</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>86</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>86</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>86</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>86</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>86</v>
+      </c>
+      <c r="B274" s="3">
+        <v>9839300490</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
King County scraper is complete for now
</commit_message>
<xml_diff>
--- a/server/Auction_Notes_2022.xlsx
+++ b/server/Auction_Notes_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcouch/Documents/CODE/react_testing/tax_auction/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2DF8D3-A8C1-4A4E-A8FC-7BFFCC26946D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E9E4DF-F0CE-A043-944C-7D7BBB94728B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
   </bookViews>
@@ -927,17 +927,17 @@
     <t>https://blue.kingcounty.com/Assessor/eRealProperty/Dashboard.aspx?ParcelNbr=</t>
   </si>
   <si>
-    <t>https://gismaps.kingcounty.gov/parcelviewer2//?pin=</t>
-  </si>
-  <si>
     <t>9/13/2023</t>
+  </si>
+  <si>
+    <t>https://gismaps.kingcounty.gov/iMap/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -965,13 +965,6 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -994,12 +987,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1318,7 +1310,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,7 +1318,7 @@
     <col min="2" max="2" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" customWidth="1"/>
     <col min="6" max="6" width="22.5" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
@@ -1389,7 +1381,7 @@
         <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>87</v>
@@ -1400,8 +1392,8 @@
       <c r="E3" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>296</v>
+      <c r="F3" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -1415,6 +1407,7 @@
     <hyperlink ref="G2" r:id="rId1" xr:uid="{A74CA47F-5F8E-444A-81BD-A214D2C9EC49}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{3456EF92-C537-B04F-B24A-4963B3B8DF33}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{20A4526F-F7E4-874C-B6C1-AD92A24BF129}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{77D76FDA-6321-1942-88B8-5F7FFA2C088C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1424,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45ED94-1D31-3149-A41C-8E0A68424B78}">
   <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:B274"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated chromedriver to 119
</commit_message>
<xml_diff>
--- a/server/Auction_Notes_2022.xlsx
+++ b/server/Auction_Notes_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcouch/Documents/CODE/react_testing/tax_auction/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E327A4-4573-E649-B4D6-92647437C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D280335-3777-CC4E-8CF2-7F07FA5E3E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{ABD64F83-5226-2944-B612-CC24CCE53FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="AuctionNotes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="309">
   <si>
     <t>COUNTY</t>
   </si>
@@ -1342,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8B109A-2724-4740-B131-3DE7DE546852}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1504,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45ED94-1D31-3149-A41C-8E0A68424B78}">
-  <dimension ref="A1:G278"/>
+  <dimension ref="A1:G318"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="D306" sqref="D306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4580,6 +4580,446 @@
         <v>305</v>
       </c>
     </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>298</v>
+      </c>
+      <c r="B279">
+        <v>319122025</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>298</v>
+      </c>
+      <c r="B280">
+        <v>319262013</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>298</v>
+      </c>
+      <c r="B281">
+        <v>319262020</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>298</v>
+      </c>
+      <c r="B282">
+        <v>518012029</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>298</v>
+      </c>
+      <c r="B283">
+        <v>518185010</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>298</v>
+      </c>
+      <c r="B284">
+        <v>520172039</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>298</v>
+      </c>
+      <c r="B285">
+        <v>2580000072</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>298</v>
+      </c>
+      <c r="B286">
+        <v>2930000383</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>298</v>
+      </c>
+      <c r="B287">
+        <v>3460000800</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>298</v>
+      </c>
+      <c r="B288">
+        <v>3615220620</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>298</v>
+      </c>
+      <c r="B289">
+        <v>4015200168</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>298</v>
+      </c>
+      <c r="B290">
+        <v>4885100520</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>298</v>
+      </c>
+      <c r="B291">
+        <v>5001930210</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>298</v>
+      </c>
+      <c r="B292">
+        <v>5002450140</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>298</v>
+      </c>
+      <c r="B293">
+        <v>5002450160</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>298</v>
+      </c>
+      <c r="B294">
+        <v>5002520560</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>298</v>
+      </c>
+      <c r="B295">
+        <v>5003370030</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>298</v>
+      </c>
+      <c r="B296">
+        <v>5017200560</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>298</v>
+      </c>
+      <c r="B297">
+        <v>5017201210</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>298</v>
+      </c>
+      <c r="B298">
+        <v>5017860320</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>298</v>
+      </c>
+      <c r="B299">
+        <v>5017860840</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>298</v>
+      </c>
+      <c r="B300">
+        <v>5017880530</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>298</v>
+      </c>
+      <c r="B301">
+        <v>5018040540</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>298</v>
+      </c>
+      <c r="B302">
+        <v>5018041090</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>298</v>
+      </c>
+      <c r="B303">
+        <v>5018060620</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>298</v>
+      </c>
+      <c r="B304">
+        <v>5018061020</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>298</v>
+      </c>
+      <c r="B305">
+        <v>5018061030</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>298</v>
+      </c>
+      <c r="B306">
+        <v>5018120020</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>298</v>
+      </c>
+      <c r="B307">
+        <v>5018160430</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>298</v>
+      </c>
+      <c r="B308">
+        <v>5545000290</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>298</v>
+      </c>
+      <c r="B309">
+        <v>5665000023</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>298</v>
+      </c>
+      <c r="B310">
+        <v>5670400422</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>298</v>
+      </c>
+      <c r="B311">
+        <v>5670400480</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>298</v>
+      </c>
+      <c r="B312">
+        <v>5670400560</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>298</v>
+      </c>
+      <c r="B313">
+        <v>5820000041</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>298</v>
+      </c>
+      <c r="B314">
+        <v>6762000810</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>298</v>
+      </c>
+      <c r="B315">
+        <v>6995100741</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>298</v>
+      </c>
+      <c r="B316">
+        <v>7470031250</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>298</v>
+      </c>
+      <c r="B317">
+        <v>7697000330</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>298</v>
+      </c>
+      <c r="B318">
+        <v>7755000853</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>